<commit_message>
[update 1] advanced py calculations
</commit_message>
<xml_diff>
--- a/rgr2/rgr2.xlsx
+++ b/rgr2/rgr2.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="F" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="l" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="h" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="w" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="F" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="l" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="h" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="w" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,14 +416,103 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B1" t="n">
+        <v>2.279202279202279e-06</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2.329851218740108e-06</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.380500158277936e-06</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.431149097815764e-06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2.481798037353593e-06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.532446976891421e-06</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2.58309591642925e-06</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.633744855967078e-06</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.684393795504906e-06</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.735042735042735e-06</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2.785691674580564e-06</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -448,7 +536,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>9.071999999999999e-28</v>
+        <v>1.846153846153847e-06</v>
       </c>
     </row>
     <row r="2">
@@ -456,7 +544,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>9.273599999999997e-28</v>
+        <v>1.971986071541628e-06</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +552,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>9.475199999999996e-28</v>
+        <v>2.103409939854384e-06</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +560,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>9.676799999999998e-28</v>
+        <v>2.240547008547009e-06</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +568,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>9.878399999999997e-28</v>
+        <v>2.383518835074391e-06</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>1.008e-27</v>
+        <v>2.532446976891422e-06</v>
       </c>
     </row>
     <row r="7">
@@ -496,7 +584,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>1.02816e-27</v>
+        <v>2.687452991452993e-06</v>
       </c>
     </row>
     <row r="8">
@@ -504,7 +592,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>1.04832e-27</v>
+        <v>2.848658436213993e-06</v>
       </c>
     </row>
     <row r="9">
@@ -512,7 +600,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>1.06848e-27</v>
+        <v>3.016184868629315e-06</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +608,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>1.08864e-27</v>
+        <v>3.190153846153848e-06</v>
       </c>
     </row>
     <row r="11">
@@ -528,7 +616,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>1.1088e-27</v>
+        <v>3.370686926242484e-06</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +643,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>7.34832e-28</v>
+        <v>3.473864165831854e-06</v>
       </c>
     </row>
     <row r="2">
@@ -563,7 +651,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>7.849175039999999e-28</v>
+        <v>3.252197256014503e-06</v>
       </c>
     </row>
     <row r="3">
@@ -571,7 +659,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>8.372286719999996e-28</v>
+        <v>3.04899561861464e-06</v>
       </c>
     </row>
     <row r="4">
@@ -579,7 +667,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>8.918138879999997e-28</v>
+        <v>2.862375869063113e-06</v>
       </c>
     </row>
     <row r="5">
@@ -587,7 +675,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>9.487215359999999e-28</v>
+        <v>2.690680516718609e-06</v>
       </c>
     </row>
     <row r="6">
@@ -595,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>1.008e-27</v>
+        <v>2.532446976891422e-06</v>
       </c>
     </row>
     <row r="7">
@@ -603,7 +691,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>1.069697664e-27</v>
+        <v>2.386381347380929e-06</v>
       </c>
     </row>
     <row r="8">
@@ -611,7 +699,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>1.133862912e-27</v>
+        <v>2.251336140983639e-06</v>
       </c>
     </row>
     <row r="9">
@@ -619,7 +707,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>1.200544128e-27</v>
+        <v>2.126291315054895e-06</v>
       </c>
     </row>
     <row r="10">
@@ -627,7 +715,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>1.269789696e-27</v>
+        <v>2.010338058930471e-06</v>
       </c>
     </row>
     <row r="11">
@@ -635,7 +723,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>1.341648e-27</v>
+        <v>1.90266489623698e-06</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +750,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>0.005758917323543174</v>
+        <v>2.813829974323802e-06</v>
       </c>
     </row>
     <row r="2">
@@ -670,7 +758,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>0.005391441410247716</v>
+        <v>2.752659757490676e-06</v>
       </c>
     </row>
     <row r="3">
@@ -678,7 +766,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>0.005054576934859058</v>
+        <v>2.694092528607896e-06</v>
       </c>
     </row>
     <row r="4">
@@ -686,7 +774,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>0.004745201652089408</v>
+        <v>2.637965600928564e-06</v>
       </c>
     </row>
     <row r="5">
@@ -694,7 +782,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>0.004460567800048209</v>
+        <v>2.584129568256553e-06</v>
       </c>
     </row>
     <row r="6">
@@ -702,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0.004198250728862975</v>
+        <v>2.532446976891422e-06</v>
       </c>
     </row>
     <row r="7">
@@ -710,7 +798,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003956105427835989</v>
+        <v>2.482791153815119e-06</v>
       </c>
     </row>
     <row r="8">
@@ -718,7 +806,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>0.003732229610746699</v>
+        <v>2.435045170087906e-06</v>
       </c>
     </row>
     <row r="9">
@@ -726,7 +814,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003524932266957768</v>
+        <v>2.389100921595681e-06</v>
       </c>
     </row>
     <row r="10">
@@ -734,7 +822,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>0.003332706784457855</v>
+        <v>2.344858311936501e-06</v>
       </c>
     </row>
     <row r="11">
@@ -742,114 +830,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003154207910490588</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="B1" t="n">
-        <v>1.12e-27</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1.095652173913043e-27</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1.072340425531915e-27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1.05e-27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1.028571428571428e-27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1.008e-27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9.882352941176469e-28</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="B8" t="n">
-        <v>9.692307692307689e-28</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9.509433962264148e-28</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9.33333333333333e-28</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B11" t="n">
-        <v>9.163636363636361e-28</v>
+        <v>2.302224524446747e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[update 2] minor changes
</commit_message>
<xml_diff>
--- a/rgr2/rgr2.xlsx
+++ b/rgr2/rgr2.xlsx
@@ -429,7 +429,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>2.279202279202279e-06</v>
+        <v>0.0001685003698224852</v>
       </c>
     </row>
     <row r="2">
@@ -437,7 +437,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>2.329851218740108e-06</v>
+        <v>0.0001722448224852071</v>
       </c>
     </row>
     <row r="3">
@@ -445,7 +445,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>2.380500158277936e-06</v>
+        <v>0.000175989275147929</v>
       </c>
     </row>
     <row r="4">
@@ -453,7 +453,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>2.431149097815764e-06</v>
+        <v>0.0001797337278106509</v>
       </c>
     </row>
     <row r="5">
@@ -461,7 +461,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>2.481798037353593e-06</v>
+        <v>0.0001834781804733728</v>
       </c>
     </row>
     <row r="6">
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>2.532446976891421e-06</v>
+        <v>0.0001872226331360947</v>
       </c>
     </row>
     <row r="7">
@@ -477,7 +477,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>2.58309591642925e-06</v>
+        <v>0.0001909670857988166</v>
       </c>
     </row>
     <row r="8">
@@ -485,7 +485,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>2.633744855967078e-06</v>
+        <v>0.0001947115384615385</v>
       </c>
     </row>
     <row r="9">
@@ -493,7 +493,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>2.684393795504906e-06</v>
+        <v>0.0001984559911242604</v>
       </c>
     </row>
     <row r="10">
@@ -501,7 +501,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>2.735042735042735e-06</v>
+        <v>0.0002022004437869823</v>
       </c>
     </row>
     <row r="11">
@@ -509,7 +509,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>2.785691674580564e-06</v>
+        <v>0.0002059448964497042</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +536,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>1.846153846153847e-06</v>
+        <v>0.0001364852995562131</v>
       </c>
     </row>
     <row r="2">
@@ -544,7 +544,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>1.971986071541628e-06</v>
+        <v>0.0001457880177514793</v>
       </c>
     </row>
     <row r="3">
@@ -552,7 +552,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>2.103409939854384e-06</v>
+        <v>0.00015550412352071</v>
       </c>
     </row>
     <row r="4">
@@ -560,7 +560,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>2.240547008547009e-06</v>
+        <v>0.0001656426035502958</v>
       </c>
     </row>
     <row r="5">
@@ -568,7 +568,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>2.383518835074391e-06</v>
+        <v>0.0001762124445266272</v>
       </c>
     </row>
     <row r="6">
@@ -576,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>2.532446976891422e-06</v>
+        <v>0.0001872226331360947</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>2.687452991452993e-06</v>
+        <v>0.0001986821560650887</v>
       </c>
     </row>
     <row r="8">
@@ -592,7 +592,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>2.848658436213993e-06</v>
+        <v>0.0002106</v>
       </c>
     </row>
     <row r="9">
@@ -600,7 +600,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>3.016184868629315e-06</v>
+        <v>0.0002229851516272189</v>
       </c>
     </row>
     <row r="10">
@@ -608,7 +608,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>3.190153846153848e-06</v>
+        <v>0.0002358465976331362</v>
       </c>
     </row>
     <row r="11">
@@ -616,7 +616,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>3.370686926242484e-06</v>
+        <v>0.0002491933247041421</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +643,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>3.473864165831854e-06</v>
+        <v>0.0002568211702827087</v>
       </c>
     </row>
     <row r="2">
@@ -651,7 +651,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>3.252197256014503e-06</v>
+        <v>0.0002404334382141431</v>
       </c>
     </row>
     <row r="3">
@@ -659,7 +659,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>3.04899561861464e-06</v>
+        <v>0.000225410835190775</v>
       </c>
     </row>
     <row r="4">
@@ -667,7 +667,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>2.862375869063113e-06</v>
+        <v>0.0002116141234629253</v>
       </c>
     </row>
     <row r="5">
@@ -675,7 +675,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>2.690680516718609e-06</v>
+        <v>0.0001989207655144696</v>
       </c>
     </row>
     <row r="6">
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>2.532446976891422e-06</v>
+        <v>0.0001872226331360946</v>
       </c>
     </row>
     <row r="7">
@@ -691,7 +691,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>2.386381347380929e-06</v>
+        <v>0.0001764240687368495</v>
       </c>
     </row>
     <row r="8">
@@ -699,7 +699,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>2.251336140983639e-06</v>
+        <v>0.0001664402391187687</v>
       </c>
     </row>
     <row r="9">
@@ -707,7 +707,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>2.126291315054895e-06</v>
+        <v>0.0001571957330011475</v>
       </c>
     </row>
     <row r="10">
@@ -715,7 +715,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>2.010338058930471e-06</v>
+        <v>0.0001486233624321231</v>
       </c>
     </row>
     <row r="11">
@@ -723,7 +723,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>1.90266489623698e-06</v>
+        <v>0.0001406631353389141</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +750,7 @@
         <v>0.9</v>
       </c>
       <c r="B1" t="n">
-        <v>2.813829974323802e-06</v>
+        <v>0.0002080251479289941</v>
       </c>
     </row>
     <row r="2">
@@ -758,7 +758,7 @@
         <v>0.92</v>
       </c>
       <c r="B2" t="n">
-        <v>2.752659757490676e-06</v>
+        <v>0.0002035028621044507</v>
       </c>
     </row>
     <row r="3">
@@ -766,7 +766,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>2.694092528607896e-06</v>
+        <v>0.0001991730139745688</v>
       </c>
     </row>
     <row r="4">
@@ -774,7 +774,7 @@
         <v>0.96</v>
       </c>
       <c r="B4" t="n">
-        <v>2.637965600928564e-06</v>
+        <v>0.000195023576183432</v>
       </c>
     </row>
     <row r="5">
@@ -782,7 +782,7 @@
         <v>0.98</v>
       </c>
       <c r="B5" t="n">
-        <v>2.584129568256553e-06</v>
+        <v>0.0001910435032000966</v>
       </c>
     </row>
     <row r="6">
@@ -790,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>2.532446976891422e-06</v>
+        <v>0.0001872226331360947</v>
       </c>
     </row>
     <row r="7">
@@ -798,7 +798,7 @@
         <v>1.02</v>
       </c>
       <c r="B7" t="n">
-        <v>2.482791153815119e-06</v>
+        <v>0.0001835516011138183</v>
       </c>
     </row>
     <row r="8">
@@ -806,7 +806,7 @@
         <v>1.04</v>
       </c>
       <c r="B8" t="n">
-        <v>2.435045170087906e-06</v>
+        <v>0.0001800217626308603</v>
       </c>
     </row>
     <row r="9">
@@ -814,7 +814,7 @@
         <v>1.06</v>
       </c>
       <c r="B9" t="n">
-        <v>2.389100921595681e-06</v>
+        <v>0.0001766251256000893</v>
       </c>
     </row>
     <row r="10">
@@ -822,7 +822,7 @@
         <v>1.08</v>
       </c>
       <c r="B10" t="n">
-        <v>2.344858311936501e-06</v>
+        <v>0.0001733542899408284</v>
       </c>
     </row>
     <row r="11">
@@ -830,7 +830,7 @@
         <v>1.1</v>
       </c>
       <c r="B11" t="n">
-        <v>2.302224524446747e-06</v>
+        <v>0.0001702023937600861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>